<commit_message>
rename RORLocationComment to RORComment 50bff9d3c395325b4b55eaf99207bb8fa7dbcdd2
</commit_message>
<xml_diff>
--- a/sg/ajouter-le-champ-commentaire/ig/StructureDefinition-ror-location.xlsx
+++ b/sg/ajouter-le-champ-commentaire/ig/StructureDefinition-ror-location.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-14T14:38:25+00:00</t>
+    <t>2025-10-15T15:37:16+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -723,13 +723,13 @@
     <t>Extension créée dans le cadre du ROR qui correspond à la date de création (dans le ROR régional) présente dans les métadonnées.</t>
   </si>
   <si>
-    <t>Location.extension:ror-location-comment</t>
-  </si>
-  <si>
-    <t>ror-location-comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/ror/StructureDefinition/ror-location-comment}
+    <t>Location.extension:ror-comment</t>
+  </si>
+  <si>
+    <t>ror-comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/ror/StructureDefinition/ror-comment}
 </t>
   </si>
   <si>

</xml_diff>